<commit_message>
Adding dynamic functionality, enhancing frontend interaction
</commit_message>
<xml_diff>
--- a/www/UploadedFiles/TeleTech.xlsx
+++ b/www/UploadedFiles/TeleTech.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\www\UploadedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TeleTech1" sheetId="1" r:id="rId1"/>
+    <sheet name="TeleTech 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>S.NO.</t>
   </si>
@@ -75,6 +76,12 @@
   </si>
   <si>
     <t>P3</t>
+  </si>
+  <si>
+    <t>123.1.2.40</t>
+  </si>
+  <si>
+    <t>123.1.2.41</t>
   </si>
 </sst>
 </file>
@@ -394,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,4 +492,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>